<commit_message>
ai lab 4 done
</commit_message>
<xml_diff>
--- a/stqa/1032190087_HrishikeshVaze_STQALab1.xlsx
+++ b/stqa/1032190087_HrishikeshVaze_STQALab1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\code\SEM7\stqa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7543781B-FA4B-42B5-904D-3F328B23BA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC77A6E7-454F-4D43-9310-A3381605F2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{D0AB56E0-3E16-4BA0-9853-B655099E2F5B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{D0AB56E0-3E16-4BA0-9853-B655099E2F5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -573,6 +573,281 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3246120</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5B16126-71C0-658B-8166-24CE0A9BB9A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3581400" y="4069080"/>
+          <a:ext cx="7772400" cy="4371975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3604260</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E6037DE-73AA-61FB-C46A-F4D3DD47ED6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3939540" y="3878580"/>
+          <a:ext cx="7772400" cy="4371975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3474720</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DB4FFFD-B765-6DDD-639A-DA2E2E6AB95B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3810000" y="3870960"/>
+          <a:ext cx="7772400" cy="4371975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>807720</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>165735</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0A89DB-A4F0-ECD0-CA65-1A039A1AB672}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3962400" y="4404360"/>
+          <a:ext cx="7772400" cy="4371975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>815340</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>13335</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{340CC9BB-4F19-9D23-C84C-0195C3EAB7F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3970020" y="4983480"/>
+          <a:ext cx="7772400" cy="4371975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -874,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC62317-034F-4E50-9DEC-4519F5259324}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1086,6 +1361,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1093,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577838E0-96BC-4C1C-B363-C866B8021FFD}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,6 +1557,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1288,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59A2AAF-D4B1-46D2-B935-C851EAE53122}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,6 +1753,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1483,8 +1761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0157112E-5CB2-4E17-B609-D9AA66954696}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1694,6 +1972,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1701,8 +1980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D5AFB5-D12F-424A-A0AC-6C3DA5A5BEF6}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1958,5 +2237,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
done with ai lab 4
</commit_message>
<xml_diff>
--- a/stqa/1032190087_HrishikeshVaze_STQALab1.xlsx
+++ b/stqa/1032190087_HrishikeshVaze_STQALab1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\code\SEM7\stqa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC77A6E7-454F-4D43-9310-A3381605F2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE2E455-45F9-4F00-86F5-A3CA6B10BD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{D0AB56E0-3E16-4BA0-9853-B655099E2F5B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D0AB56E0-3E16-4BA0-9853-B655099E2F5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC62317-034F-4E50-9DEC-4519F5259324}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1369,7 +1369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577838E0-96BC-4C1C-B363-C866B8021FFD}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1565,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59A2AAF-D4B1-46D2-B935-C851EAE53122}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1761,7 +1761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0157112E-5CB2-4E17-B609-D9AA66954696}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1980,7 +1980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D5AFB5-D12F-424A-A0AC-6C3DA5A5BEF6}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>

</xml_diff>